<commit_message>
docs: actualizacion en contenido de documentos
</commit_message>
<xml_diff>
--- a/documentos/01. INICIO/20251002_Registro-de-Interesados_v1.1.0.xlsx
+++ b/documentos/01. INICIO/20251002_Registro-de-Interesados_v1.1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185068B9-1CE3-41E2-A40D-442F6D26B9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C70F08-38FC-43FD-9ECB-698C1B441606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,12 +11,25 @@
     <sheet name="Stakeholders" sheetId="1" r:id="rId1"/>
     <sheet name="Comunicación" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
   <si>
     <t>ID</t>
   </si>
@@ -285,9 +298,6 @@
     <t>72913436@continental.edu.pe</t>
   </si>
   <si>
-    <t>Comunicación Diferenciada por Grupo</t>
-  </si>
-  <si>
     <t>Grupo</t>
   </si>
   <si>
@@ -397,6 +407,9 @@
   </si>
   <si>
     <t>Progress del sprint, impedimentos y decisiones de priorización</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN DIFERENCIADA POR GRUPO</t>
   </si>
 </sst>
 </file>
@@ -625,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -664,9 +677,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -714,6 +724,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -722,6 +741,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,7 +1055,7 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1063,7 @@
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
@@ -1055,26 +1080,24 @@
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="30" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="32"/>
-      <c r="F3" s="31"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
@@ -1082,23 +1105,23 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="28" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="25" t="s">
+      <c r="G6" s="28"/>
+      <c r="H6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
@@ -1173,20 +1196,20 @@
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="16" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="21" t="s">
         <v>42</v>
       </c>
       <c r="L9" s="14" t="s">
@@ -1206,20 +1229,20 @@
       <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="16"/>
+      <c r="G10" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="21" t="s">
         <v>26</v>
       </c>
       <c r="L10" s="13" t="s">
@@ -1239,22 +1262,22 @@
       <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>76</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="21" t="s">
         <v>39</v>
       </c>
       <c r="L11" s="13" t="s">
@@ -1274,22 +1297,22 @@
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="37" t="s">
         <v>48</v>
       </c>
       <c r="L12" s="13" t="s">
@@ -1309,22 +1332,22 @@
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="37" t="s">
         <v>50</v>
       </c>
       <c r="L13" s="13" t="s">
@@ -1344,22 +1367,22 @@
       <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="37" t="s">
         <v>50</v>
       </c>
       <c r="L14" s="13" t="s">
@@ -1379,22 +1402,22 @@
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="15" t="s">
         <v>78</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="37" t="s">
         <v>59</v>
       </c>
       <c r="L15" s="13" t="s">
@@ -1414,22 +1437,22 @@
       <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="37" t="s">
         <v>62</v>
       </c>
       <c r="L16" s="13" t="s">
@@ -1449,22 +1472,22 @@
       <c r="E17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="37" t="s">
         <v>65</v>
       </c>
       <c r="L17" s="13" t="s">
@@ -1484,22 +1507,22 @@
       <c r="E18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="K18" s="38" t="s">
         <v>30</v>
       </c>
       <c r="L18" s="13" t="s">
@@ -1519,22 +1542,22 @@
       <c r="E19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="38" t="s">
         <v>32</v>
       </c>
       <c r="L19" s="13" t="s">
@@ -1587,7 +1610,7 @@
   <dimension ref="B1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,170 +1626,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
-        <v>87</v>
+      <c r="B1" s="18" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="22">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="20" t="s">
+      <c r="D4" s="23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
-        <v>1</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="22">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="22">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="H4" s="24" t="s">
+      <c r="F6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="22">
+        <v>5</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="22">
+        <v>6</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
-        <v>2</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
-        <v>4</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
-        <v>5</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
-        <v>6</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="24" t="s">
+    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="22">
+        <v>7</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="24" t="s">
+      <c r="E9" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H9" s="23" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="23">
-        <v>7</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>